<commit_message>
v0.1: created three endpoints for upload, similarity check and document search
</commit_message>
<xml_diff>
--- a/Estimates.CSV (Challenges) - Sheet1.xlsx
+++ b/Estimates.CSV (Challenges) - Sheet1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>Story</t>
   </si>
@@ -58,10 +58,19 @@
     <t>Setup ChromaDB</t>
   </si>
   <si>
+    <t>10 minutes</t>
+  </si>
+  <si>
+    <t>Installed the required libraries and initiated the DB</t>
+  </si>
+  <si>
     <t>Embeddings</t>
   </si>
   <si>
-    <t>Create embeddings using LLM</t>
+    <t>Create embeddings using LLM/Sentence Transformer</t>
+  </si>
+  <si>
+    <t>Created two approaches to get the embedding. One with Open AI embedding model and the another with Sentence Transformer. Since Open AI's embedding model is paid, we can go with the Sentence Transformer which is free of cost.</t>
   </si>
   <si>
     <t>ChatBot</t>
@@ -76,12 +85,18 @@
     <t xml:space="preserve"> Check the similarity of the embeddings using Cosine similarity</t>
   </si>
   <si>
+    <t>ChromaDB's default way of checking similarity is using Cosine Similarity.</t>
+  </si>
+  <si>
     <t>Final output</t>
   </si>
   <si>
     <t>Get the final output from after similarity check</t>
   </si>
   <si>
+    <t>Done in Postman</t>
+  </si>
+  <si>
     <t>Generate summary</t>
   </si>
   <si>
@@ -94,6 +109,9 @@
     <t>Endpoints for uploading and storing chunks</t>
   </si>
   <si>
+    <t>For creating and testing using Postman</t>
+  </si>
+  <si>
     <t>Build API for similarity check</t>
   </si>
   <si>
@@ -104,6 +122,12 @@
   </si>
   <si>
     <t>endpoint to get details of specific journal when requested</t>
+  </si>
+  <si>
+    <t>30 minutes</t>
+  </si>
+  <si>
+    <t>Here I was facing some issues to get the details of the specific source_doc_id requested. But was able to debug it later.</t>
   </si>
 </sst>
 </file>
@@ -555,15 +579,19 @@
       <c r="D4" s="4">
         <v>2</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C5" s="4">
         <v>2</v>
@@ -571,15 +599,19 @@
       <c r="D5" s="4">
         <v>3</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C6" s="4">
         <v>2</v>
@@ -592,10 +624,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C7" s="4">
         <v>2</v>
@@ -603,15 +635,19 @@
       <c r="D7" s="4">
         <v>3</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
@@ -619,15 +655,19 @@
       <c r="D8" s="4">
         <v>3</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C9" s="4">
         <v>2</v>
@@ -640,10 +680,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
@@ -651,15 +691,19 @@
       <c r="D10" s="4">
         <v>2</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
@@ -667,15 +711,19 @@
       <c r="D11" s="4">
         <v>2</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C12" s="4">
         <v>1</v>
@@ -683,8 +731,12 @@
       <c r="D12" s="4">
         <v>2</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
v0.2: Updated upload, similarity_search, and searching documents endpoint
</commit_message>
<xml_diff>
--- a/Estimates.CSV (Challenges) - Sheet1.xlsx
+++ b/Estimates.CSV (Challenges) - Sheet1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>Story</t>
   </si>
@@ -109,7 +109,10 @@
     <t>Endpoints for uploading and storing chunks</t>
   </si>
   <si>
-    <t>For creating and testing using Postman</t>
+    <t>45 minutes</t>
+  </si>
+  <si>
+    <t>For creating and testing using Postman, Made changes in uploading json from file url and also using chunks</t>
   </si>
   <si>
     <t>Build API for similarity check</t>
@@ -118,6 +121,9 @@
     <t>Similarity search endpoint to query documents</t>
   </si>
   <si>
+    <t>For creating and testing using Postman, Made changes in the response which took some time to debug</t>
+  </si>
+  <si>
     <t>Build API for get</t>
   </si>
   <si>
@@ -127,7 +133,7 @@
     <t>30 minutes</t>
   </si>
   <si>
-    <t>Here I was facing some issues to get the details of the specific source_doc_id requested. But was able to debug it later.</t>
+    <t/>
   </si>
 </sst>
 </file>
@@ -177,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -189,6 +195,9 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -502,12 +511,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="52.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="21.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="21.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="52.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="21.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="18.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="21.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -692,18 +701,18 @@
         <v>2</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
@@ -712,18 +721,18 @@
         <v>2</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C12" s="4">
         <v>1</v>
@@ -732,10 +741,10 @@
         <v>2</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v0.3: created chatbot for user query, answers, citations and chart
</commit_message>
<xml_diff>
--- a/Estimates.CSV (Challenges) - Sheet1.xlsx
+++ b/Estimates.CSV (Challenges) - Sheet1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t>Story</t>
   </si>
@@ -79,6 +79,12 @@
     <t>Create ChatBot to give user query</t>
   </si>
   <si>
+    <t>1 hour</t>
+  </si>
+  <si>
+    <t>The chatbot answers research questions based on semantic search from uploaded journal chunks.  It shows the answer, top 5 citations with metadata and links, and a usage chart. The answer is LLM generated by understanding the context and rewriting in its own words.</t>
+  </si>
+  <si>
     <t>Similarity check</t>
   </si>
   <si>
@@ -100,7 +106,7 @@
     <t>Generate summary</t>
   </si>
   <si>
-    <t>Generate the summary of the output</t>
+    <t>Generate the summary of the user input</t>
   </si>
   <si>
     <t>Build API for upload</t>
@@ -628,15 +634,19 @@
       <c r="D6" s="4">
         <v>3</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C7" s="4">
         <v>2</v>
@@ -648,15 +658,15 @@
         <v>14</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
@@ -668,15 +678,15 @@
         <v>14</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C9" s="4">
         <v>2</v>
@@ -689,10 +699,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
@@ -701,18 +711,18 @@
         <v>2</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
@@ -721,18 +731,18 @@
         <v>2</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C12" s="4">
         <v>1</v>
@@ -741,10 +751,10 @@
         <v>2</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v0.5: Added Ingestion pipeline pseudocode and its short explanation.
</commit_message>
<xml_diff>
--- a/Estimates.CSV (Challenges) - Sheet1.xlsx
+++ b/Estimates.CSV (Challenges) - Sheet1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>Story</t>
   </si>
@@ -40,6 +40,12 @@
     <t>Write ingestion pseudocode and architecture plan</t>
   </si>
   <si>
+    <t>30 minutes</t>
+  </si>
+  <si>
+    <t>Pseudo code for ingestion pipeline and explanation is give in the ingestion_pipeline markdown file.</t>
+  </si>
+  <si>
     <t>Project setup</t>
   </si>
   <si>
@@ -134,9 +140,6 @@
   </si>
   <si>
     <t>endpoint to get details of specific journal when requested</t>
-  </si>
-  <si>
-    <t>30 minutes</t>
   </si>
   <si>
     <t/>
@@ -558,15 +561,19 @@
       <c r="D2" s="2">
         <v>1.5</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2">
         <v>0.5</v>
@@ -575,18 +582,18 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" s="4">
         <v>1</v>
@@ -595,18 +602,18 @@
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5" s="4">
         <v>2</v>
@@ -615,18 +622,18 @@
         <v>3</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C6" s="4">
         <v>2</v>
@@ -635,18 +642,18 @@
         <v>3</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C7" s="4">
         <v>2</v>
@@ -655,18 +662,18 @@
         <v>3</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
@@ -675,18 +682,18 @@
         <v>3</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C9" s="4">
         <v>2</v>
@@ -699,10 +706,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
@@ -711,18 +718,18 @@
         <v>2</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
@@ -731,18 +738,18 @@
         <v>2</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C12" s="4">
         <v>1</v>
@@ -751,10 +758,10 @@
         <v>2</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v0.9: Added summarizing and comapring documents
</commit_message>
<xml_diff>
--- a/Estimates.CSV (Challenges) - Sheet1.xlsx
+++ b/Estimates.CSV (Challenges) - Sheet1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>Story</t>
   </si>
@@ -40,79 +40,91 @@
     <t>Write ingestion pseudocode and architecture plan</t>
   </si>
   <si>
+    <t>1 hour</t>
+  </si>
+  <si>
+    <t>Pseudo code for ingestion pipeline and explanation is give in the ingestion_pipeline markdown file.</t>
+  </si>
+  <si>
+    <t>Project setup</t>
+  </si>
+  <si>
+    <t>Create github repository and setup project</t>
+  </si>
+  <si>
+    <t>15 minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created basic structure of the project </t>
+  </si>
+  <si>
+    <t>VectorDB setup</t>
+  </si>
+  <si>
+    <t>Setup ChromaDB</t>
+  </si>
+  <si>
+    <t>10 minutes</t>
+  </si>
+  <si>
+    <t>Installed the required libraries and initiated the DB</t>
+  </si>
+  <si>
+    <t>Embeddings</t>
+  </si>
+  <si>
+    <t>Create embeddings using LLM/Sentence Transformer</t>
+  </si>
+  <si>
+    <t>Created two approaches to get the embedding. One with Open AI embedding model and the another with Sentence Transformer. Since Open AI's embedding model is paid, we can go with the Sentence Transformer which is free of cost.</t>
+  </si>
+  <si>
+    <t>ChatBot</t>
+  </si>
+  <si>
+    <t>Create ChatBot to give user query</t>
+  </si>
+  <si>
+    <t>The chatbot answers research questions based on semantic search from uploaded journal chunks.  It shows the answer, top 5 citations with metadata and links, and a usage chart. The answer is LLM generated by understanding the context and rewriting in its own words.</t>
+  </si>
+  <si>
+    <t>Similarity check</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Check the similarity of the embeddings using Cosine similarity</t>
+  </si>
+  <si>
+    <t>ChromaDB's default way of checking similarity is using Cosine Similarity.</t>
+  </si>
+  <si>
+    <t>Final output</t>
+  </si>
+  <si>
+    <t>Get the final output from after similarity check</t>
+  </si>
+  <si>
+    <t>Done in Postman</t>
+  </si>
+  <si>
+    <t>Generate summary</t>
+  </si>
+  <si>
+    <t>Generate the summary of the user input document</t>
+  </si>
+  <si>
     <t>30 minutes</t>
   </si>
   <si>
-    <t>Pseudo code for ingestion pipeline and explanation is give in the ingestion_pipeline markdown file.</t>
-  </si>
-  <si>
-    <t>Project setup</t>
-  </si>
-  <si>
-    <t>Create github repository and setup project</t>
-  </si>
-  <si>
-    <t>15 minutes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Created basic structure of the project </t>
-  </si>
-  <si>
-    <t>VectorDB setup</t>
-  </si>
-  <si>
-    <t>Setup ChromaDB</t>
-  </si>
-  <si>
-    <t>10 minutes</t>
-  </si>
-  <si>
-    <t>Installed the required libraries and initiated the DB</t>
-  </si>
-  <si>
-    <t>Embeddings</t>
-  </si>
-  <si>
-    <t>Create embeddings using LLM/Sentence Transformer</t>
-  </si>
-  <si>
-    <t>Created two approaches to get the embedding. One with Open AI embedding model and the another with Sentence Transformer. Since Open AI's embedding model is paid, we can go with the Sentence Transformer which is free of cost.</t>
-  </si>
-  <si>
-    <t>ChatBot</t>
-  </si>
-  <si>
-    <t>Create ChatBot to give user query</t>
-  </si>
-  <si>
-    <t>1 hour</t>
-  </si>
-  <si>
-    <t>The chatbot answers research questions based on semantic search from uploaded journal chunks.  It shows the answer, top 5 citations with metadata and links, and a usage chart. The answer is LLM generated by understanding the context and rewriting in its own words.</t>
-  </si>
-  <si>
-    <t>Similarity check</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Check the similarity of the embeddings using Cosine similarity</t>
-  </si>
-  <si>
-    <t>ChromaDB's default way of checking similarity is using Cosine Similarity.</t>
-  </si>
-  <si>
-    <t>Final output</t>
-  </si>
-  <si>
-    <t>Get the final output from after similarity check</t>
-  </si>
-  <si>
-    <t>Done in Postman</t>
-  </si>
-  <si>
-    <t>Generate summary</t>
-  </si>
-  <si>
-    <t>Generate the summary of the user input</t>
+    <t>It will generate the summary of the selected document with the help of Open AI's GPT</t>
+  </si>
+  <si>
+    <t>Compare documents</t>
+  </si>
+  <si>
+    <t>Compare two different documents selected by the user</t>
+  </si>
+  <si>
+    <t>It will compare the two documents selected by the user. It also uses the OpenAI's GPT</t>
   </si>
   <si>
     <t>Build API for upload</t>
@@ -142,7 +154,16 @@
     <t>endpoint to get details of specific journal when requested</t>
   </si>
   <si>
-    <t/>
+    <t>Readme.md</t>
+  </si>
+  <si>
+    <t>Creating readme.md explaining the pipeline</t>
+  </si>
+  <si>
+    <t>Extra features</t>
+  </si>
+  <si>
+    <t>Creating extra_features.md</t>
   </si>
 </sst>
 </file>
@@ -150,13 +171,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -192,22 +219,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -514,31 +553,31 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="52.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="21.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="21.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="52.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="21.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="18.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="21.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -548,221 +587,279 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>0.5</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <v>1.5</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>0.5</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="5">
         <v>1</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="5">
         <v>1</v>
       </c>
-      <c r="D4" s="4">
-        <v>2</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="4">
-        <v>2</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="C5" s="5">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5">
         <v>3</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="4">
-        <v>2</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="C6" s="5">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5">
         <v>3</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="3" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="5">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5">
+        <v>3</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="4">
-        <v>2</v>
-      </c>
-      <c r="D7" s="4">
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5">
         <v>3</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="F8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="4">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4">
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2</v>
+      </c>
+      <c r="D9" s="5">
         <v>3</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="E9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="4">
-        <v>2</v>
-      </c>
-      <c r="D9" s="4">
+      <c r="F9" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="7">
+        <v>2</v>
+      </c>
+      <c r="D10" s="7">
         <v>3</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="4">
-        <v>1</v>
-      </c>
-      <c r="D10" s="4">
-        <v>2</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="E10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="5">
         <v>1</v>
       </c>
-      <c r="D11" s="4">
-        <v>2</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="D11" s="5">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="F11" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="4">
+        <v>42</v>
+      </c>
+      <c r="C12" s="5">
         <v>1</v>
       </c>
-      <c r="D12" s="4">
-        <v>2</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="D12" s="5">
+        <v>2</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="7">
+        <v>1</v>
+      </c>
+      <c r="D13" s="7">
+        <v>2</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="7">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7">
+        <v>2</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="F14" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1</v>
+      </c>
+      <c r="D15" s="5">
+        <v>2</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>